<commit_message>
Input nome do romaneio e input de hora
</commit_message>
<xml_diff>
--- a/Romaneio.xlsx
+++ b/Romaneio.xlsx
@@ -1323,7 +1323,7 @@
       <c r="A4" s="8" t="n"/>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>DATA: 20/02/2023</t>
+          <t>DATA: 11/03/2023</t>
         </is>
       </c>
       <c r="C4" s="13" t="inlineStr">
@@ -1344,7 +1344,7 @@
     <row r="6" ht="22.5" customHeight="1">
       <c r="A6" s="14" t="inlineStr">
         <is>
-          <t xml:space="preserve">FERROTELHAS - </t>
+          <t>FERROTELHAS - BAIXADA</t>
         </is>
       </c>
       <c r="B6" s="15" t="inlineStr">
@@ -1368,7 +1368,7 @@
       <c r="B7" s="4" t="n"/>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>20/02/2023</t>
+          <t>11/03/2023</t>
         </is>
       </c>
       <c r="H7" s="7" t="n"/>
@@ -1376,43 +1376,67 @@
     <row r="8">
       <c r="A8" s="17" t="inlineStr">
         <is>
-          <t>TRELIÇA H8 - 7 MT</t>
+          <t>COLUNA PRONTA 1/4 6,3 MM 28 EST. (7 X 20 X 6MTS)</t>
         </is>
       </c>
       <c r="B8" s="26" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C8" s="6" t="n"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="17" t="inlineStr">
         <is>
+          <t>MALHA POP 3.4MM (20X20) 2X3M</t>
+        </is>
+      </c>
+      <c r="B9" s="20" t="n">
+        <v>50</v>
+      </c>
+      <c r="C9" s="6" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="17" t="inlineStr">
+        <is>
           <t>TRELIÇA H8 - 9 MT</t>
         </is>
       </c>
-      <c r="B9" s="20" t="n">
-        <v>450</v>
-      </c>
-      <c r="C9" s="6" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="17" t="n"/>
-      <c r="B10" s="10" t="n"/>
+      <c r="B10" s="10" t="n">
+        <v>100</v>
+      </c>
       <c r="C10" s="6" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="17" t="n"/>
-      <c r="B11" s="26" t="n"/>
+      <c r="A11" s="17" t="inlineStr">
+        <is>
+          <t>VERGALHÃO DOBRADO 6.3 MM 1/4 12 MT (CA50)</t>
+        </is>
+      </c>
+      <c r="B11" s="26" t="n">
+        <v>100</v>
+      </c>
       <c r="C11" s="6" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="17" t="n"/>
-      <c r="B12" s="21" t="n"/>
+      <c r="A12" s="17" t="inlineStr">
+        <is>
+          <t>VERGALHÃO DOBRADO 8,0 MM 5/16 12 MT (CA50)</t>
+        </is>
+      </c>
+      <c r="B12" s="21" t="n">
+        <v>100</v>
+      </c>
       <c r="C12" s="6" t="n"/>
     </row>
     <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="17" t="n"/>
-      <c r="B13" s="5" t="n"/>
+      <c r="A13" s="17" t="inlineStr">
+        <is>
+          <t>VERGALHÃO DOBRADO 3/16 12 MT (CA60)</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>100</v>
+      </c>
       <c r="C13" s="6" t="n"/>
     </row>
     <row r="14">

</xml_diff>